<commit_message>
added a bunch of features
</commit_message>
<xml_diff>
--- a/Resources/sampleData.xlsx
+++ b/Resources/sampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drives\Primary\Study\Uni Work\2020\S2\SWE30010\local\DP2_pass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jayden McQueen\Documents\Swinburne Work\DP2_pass\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB8EF88B-26E2-4CE6-938E-2D478B36A621}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871FB5D6-E781-4AD6-B9DC-A3CDE2D64259}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{25C7DEC9-8646-4E75-80FE-42F1C3BFF1FC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25C7DEC9-8646-4E75-80FE-42F1C3BFF1FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
   <si>
     <t>date</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>S000000025</t>
+  </si>
+  <si>
+    <t>num_in_stock</t>
   </si>
 </sst>
 </file>
@@ -316,11 +319,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
@@ -638,13 +642,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61456C4B-0DA4-410F-8D8C-E9F4C8D4A027}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -661,7 +666,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -677,8 +682,8 @@
       <c r="D2">
         <v>24.5</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>22</v>
+      <c r="E2" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -694,8 +699,8 @@
       <c r="D3">
         <v>29.95</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>22</v>
+      <c r="E3" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -711,8 +716,8 @@
       <c r="D4">
         <v>26.99</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
+      <c r="E4" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -728,8 +733,8 @@
       <c r="D5">
         <v>37.99</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>24</v>
+      <c r="E5" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -745,8 +750,8 @@
       <c r="D6">
         <v>14.99</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>24</v>
+      <c r="E6" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -762,8 +767,8 @@
       <c r="D7">
         <v>19.95</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>24</v>
+      <c r="E7" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -779,8 +784,8 @@
       <c r="D8">
         <v>96.99</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>28</v>
+      <c r="E8" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -796,13 +801,13 @@
       <c r="D9">
         <v>43.99</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>28</v>
+      <c r="E9" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1038,19 +1043,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9306E72-F658-451F-8129-6008C62CCCC2}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -1060,8 +1066,11 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -1071,8 +1080,11 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
@@ -1082,8 +1094,11 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
@@ -1093,8 +1108,11 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
@@ -1104,8 +1122,11 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -1115,8 +1136,11 @@
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
@@ -1126,8 +1150,11 @@
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
@@ -1137,8 +1164,11 @@
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -1148,8 +1178,11 @@
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
@@ -1159,8 +1192,11 @@
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
@@ -1170,8 +1206,11 @@
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -1181,8 +1220,11 @@
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
@@ -1192,8 +1234,11 @@
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
@@ -1203,8 +1248,11 @@
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
@@ -1214,8 +1262,11 @@
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
@@ -1225,8 +1276,11 @@
       <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
@@ -1236,8 +1290,11 @@
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
@@ -1247,8 +1304,11 @@
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
@@ -1258,8 +1318,11 @@
       <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
@@ -1269,8 +1332,11 @@
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>64</v>
       </c>
@@ -1280,8 +1346,11 @@
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
@@ -1291,8 +1360,11 @@
       <c r="C22" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="1">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
@@ -1302,8 +1374,11 @@
       <c r="C23" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
@@ -1313,8 +1388,11 @@
       <c r="C24" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
@@ -1324,8 +1402,11 @@
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
@@ -1334,6 +1415,9 @@
       </c>
       <c r="C26" s="1" t="s">
         <v>14</v>
+      </c>
+      <c r="D26" s="1">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "merged master to login branch"
This reverts commit 349fd5bf6161cbabc404fe2f8f7d9d49ff422c72, reversing
changes made to 51e90c6991f421690577cd67c3741317dd0911d5.
</commit_message>
<xml_diff>
--- a/Resources/sampleData.xlsx
+++ b/Resources/sampleData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jayden McQueen\Documents\Swinburne Work\DP2_pass\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Google Drives\Primary\Study\Uni Work\2020\S2\SWE30010\local\DP2_pass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871FB5D6-E781-4AD6-B9DC-A3CDE2D64259}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB8EF88B-26E2-4CE6-938E-2D478B36A621}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{25C7DEC9-8646-4E75-80FE-42F1C3BFF1FC}"/>
+    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{25C7DEC9-8646-4E75-80FE-42F1C3BFF1FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Products" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="70">
   <si>
     <t>date</t>
   </si>
@@ -246,9 +246,6 @@
   </si>
   <si>
     <t>S000000025</t>
-  </si>
-  <si>
-    <t>num_in_stock</t>
   </si>
 </sst>
 </file>
@@ -319,12 +316,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent2" xfId="1" builtinId="33"/>
@@ -642,14 +638,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61456C4B-0DA4-410F-8D8C-E9F4C8D4A027}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="55.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -666,7 +661,7 @@
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -682,8 +677,8 @@
       <c r="D2">
         <v>24.5</v>
       </c>
-      <c r="E2" s="4">
-        <v>0</v>
+      <c r="E2" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -699,8 +694,8 @@
       <c r="D3">
         <v>29.95</v>
       </c>
-      <c r="E3" s="4">
-        <v>0</v>
+      <c r="E3" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -716,8 +711,8 @@
       <c r="D4">
         <v>26.99</v>
       </c>
-      <c r="E4" s="4">
-        <v>0</v>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -733,8 +728,8 @@
       <c r="D5">
         <v>37.99</v>
       </c>
-      <c r="E5" s="4">
-        <v>0</v>
+      <c r="E5" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -750,8 +745,8 @@
       <c r="D6">
         <v>14.99</v>
       </c>
-      <c r="E6" s="4">
-        <v>0</v>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -767,8 +762,8 @@
       <c r="D7">
         <v>19.95</v>
       </c>
-      <c r="E7" s="4">
-        <v>0</v>
+      <c r="E7" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -784,8 +779,8 @@
       <c r="D8">
         <v>96.99</v>
       </c>
-      <c r="E8" s="4">
-        <v>0</v>
+      <c r="E8" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -801,13 +796,13 @@
       <c r="D9">
         <v>43.99</v>
       </c>
-      <c r="E9" s="4">
-        <v>0</v>
+      <c r="E9" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1043,20 +1038,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9306E72-F658-451F-8129-6008C62CCCC2}">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
@@ -1066,11 +1060,8 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -1080,11 +1071,8 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
@@ -1094,11 +1082,8 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>47</v>
       </c>
@@ -1108,11 +1093,8 @@
       <c r="C4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
@@ -1122,11 +1104,8 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="1">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>49</v>
       </c>
@@ -1136,11 +1115,8 @@
       <c r="C6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="1">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>50</v>
       </c>
@@ -1150,11 +1126,8 @@
       <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="1">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>51</v>
       </c>
@@ -1164,11 +1137,8 @@
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="1">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -1178,11 +1148,8 @@
       <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="1">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>53</v>
       </c>
@@ -1192,11 +1159,8 @@
       <c r="C10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>54</v>
       </c>
@@ -1206,11 +1170,8 @@
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>55</v>
       </c>
@@ -1220,11 +1181,8 @@
       <c r="C12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>56</v>
       </c>
@@ -1234,11 +1192,8 @@
       <c r="C13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="1">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>57</v>
       </c>
@@ -1248,11 +1203,8 @@
       <c r="C14" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D14" s="1">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
@@ -1262,11 +1214,8 @@
       <c r="C15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>59</v>
       </c>
@@ -1276,11 +1225,8 @@
       <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>60</v>
       </c>
@@ -1290,11 +1236,8 @@
       <c r="C17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D17" s="1">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>61</v>
       </c>
@@ -1304,11 +1247,8 @@
       <c r="C18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>62</v>
       </c>
@@ -1318,11 +1258,8 @@
       <c r="C19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>63</v>
       </c>
@@ -1332,11 +1269,8 @@
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="1">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>64</v>
       </c>
@@ -1346,11 +1280,8 @@
       <c r="C21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="1">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>65</v>
       </c>
@@ -1360,11 +1291,8 @@
       <c r="C22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="1">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>66</v>
       </c>
@@ -1374,11 +1302,8 @@
       <c r="C23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="1">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>67</v>
       </c>
@@ -1388,11 +1313,8 @@
       <c r="C24" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
@@ -1402,11 +1324,8 @@
       <c r="C25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D25" s="1">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>69</v>
       </c>
@@ -1415,9 +1334,6 @@
       </c>
       <c r="C26" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="D26" s="1">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>